<commit_message>
include version number for NINDS
</commit_message>
<xml_diff>
--- a/test/data/ninds-test.xlsx
+++ b/test/data/ninds-test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2465" uniqueCount="1062">
   <si>
     <t>Name</t>
   </si>
@@ -4045,6 +4045,9 @@
   </si>
   <si>
     <t>C06436</t>
+  </si>
+  <si>
+    <t>CDE Version</t>
   </si>
 </sst>
 </file>
@@ -4080,7 +4083,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4089,6 +4092,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4390,15 +4394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH136"/>
+  <dimension ref="A1:BI136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD136"/>
+    <sheetView tabSelected="1" topLeftCell="AJ107" workbookViewId="0">
+      <selection activeCell="BG138" sqref="BG138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4579,8 +4583,11 @@
       <c r="BH1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -4614,8 +4621,11 @@
       <c r="AW2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI2" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4652,8 +4662,11 @@
       <c r="BF3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -4696,8 +4709,11 @@
       <c r="BH4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -4752,8 +4768,11 @@
       <c r="BH5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -4808,8 +4827,11 @@
       <c r="BH6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -4858,8 +4880,11 @@
       <c r="BH7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI7" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -4908,8 +4933,11 @@
       <c r="BH8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -4958,8 +4986,11 @@
       <c r="BH9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -5008,8 +5039,11 @@
       <c r="BH10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI10" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -5058,8 +5092,11 @@
       <c r="BH11" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="12" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI11" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -5108,8 +5145,11 @@
       <c r="BH12" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="13" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI12" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -5158,8 +5198,11 @@
       <c r="BH13" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="14" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI13" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -5217,8 +5260,11 @@
       <c r="BB14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI14" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -5276,8 +5322,11 @@
       <c r="BB15" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI15" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -5332,8 +5381,11 @@
       <c r="AS16" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="17" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI16" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -5388,8 +5440,11 @@
       <c r="AS17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI17" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -5444,8 +5499,11 @@
       <c r="AS18" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI18" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -5500,8 +5558,11 @@
       <c r="AS19" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI19" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -5556,8 +5617,11 @@
       <c r="AS20" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="21" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI20" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>166</v>
       </c>
@@ -5612,8 +5676,11 @@
       <c r="AS21" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>170</v>
       </c>
@@ -5668,8 +5735,11 @@
       <c r="AS22" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI22" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>174</v>
       </c>
@@ -5724,8 +5794,11 @@
       <c r="AS23" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI23" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>178</v>
       </c>
@@ -5768,8 +5841,11 @@
       <c r="AW24" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI24" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -5812,8 +5888,11 @@
       <c r="AW25" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI25" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>190</v>
       </c>
@@ -5856,8 +5935,11 @@
       <c r="AW26" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI26" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>195</v>
       </c>
@@ -5900,8 +5982,11 @@
       <c r="AW27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI27" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>201</v>
       </c>
@@ -5962,8 +6047,11 @@
       <c r="BB28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="29" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI28" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>207</v>
       </c>
@@ -6003,8 +6091,11 @@
       <c r="AW29" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI29" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>212</v>
       </c>
@@ -6047,8 +6138,11 @@
       <c r="AW30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI30" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -6109,8 +6203,11 @@
       <c r="BB31" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI31" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>222</v>
       </c>
@@ -6153,8 +6250,11 @@
       <c r="AW32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI32" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>228</v>
       </c>
@@ -6194,8 +6294,11 @@
       <c r="AW33" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="34" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI33" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>233</v>
       </c>
@@ -6238,8 +6341,11 @@
       <c r="AW34" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="35" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI34" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>241</v>
       </c>
@@ -6282,8 +6388,11 @@
       <c r="AW35" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="36" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI35" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>247</v>
       </c>
@@ -6326,8 +6435,11 @@
       <c r="AW36" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI36" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>253</v>
       </c>
@@ -6370,8 +6482,11 @@
       <c r="AW37" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="38" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI37" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>257</v>
       </c>
@@ -6414,8 +6529,11 @@
       <c r="AW38" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="39" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI38" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>262</v>
       </c>
@@ -6476,8 +6594,11 @@
       <c r="BB39" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI39" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>267</v>
       </c>
@@ -6520,8 +6641,11 @@
       <c r="AW40" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI40" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>273</v>
       </c>
@@ -6576,8 +6700,11 @@
       <c r="BH41" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="42" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI41" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>280</v>
       </c>
@@ -6638,8 +6765,11 @@
       <c r="BH42" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="43" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI42" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>289</v>
       </c>
@@ -6694,8 +6824,11 @@
       <c r="BH43" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="44" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI43" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>298</v>
       </c>
@@ -6750,8 +6883,11 @@
       <c r="BH44" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="45" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI44" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>306</v>
       </c>
@@ -6842,8 +6978,11 @@
       <c r="BH45" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="46" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI45" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>316</v>
       </c>
@@ -6898,8 +7037,11 @@
       <c r="BH46" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="47" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI46" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>327</v>
       </c>
@@ -6951,8 +7093,11 @@
       <c r="BH47" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="48" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI47" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>339</v>
       </c>
@@ -7007,8 +7152,11 @@
       <c r="BH48" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="49" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI48" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>348</v>
       </c>
@@ -7063,8 +7211,11 @@
       <c r="BH49" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="50" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI49" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>357</v>
       </c>
@@ -7119,8 +7270,11 @@
       <c r="BH50" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="51" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI50" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>366</v>
       </c>
@@ -7175,8 +7329,11 @@
       <c r="BH51" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="52" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI51" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>375</v>
       </c>
@@ -7231,8 +7388,11 @@
       <c r="BH52" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="53" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI52" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>384</v>
       </c>
@@ -7287,8 +7447,11 @@
       <c r="BH53" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="54" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI53" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>392</v>
       </c>
@@ -7343,8 +7506,11 @@
       <c r="BH54" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="55" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI54" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>401</v>
       </c>
@@ -7399,8 +7565,11 @@
       <c r="BH55" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="56" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI55" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>410</v>
       </c>
@@ -7455,8 +7624,11 @@
       <c r="BH56" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="57" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI56" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>419</v>
       </c>
@@ -7511,8 +7683,11 @@
       <c r="BH57" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="58" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI57" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>428</v>
       </c>
@@ -7564,8 +7739,11 @@
       <c r="BH58" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="59" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI58" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>437</v>
       </c>
@@ -7617,8 +7795,11 @@
       <c r="BH59" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="60" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI59" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>447</v>
       </c>
@@ -7679,8 +7860,11 @@
       <c r="BH60" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="61" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI60" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>456</v>
       </c>
@@ -7747,8 +7931,11 @@
       <c r="BH61" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="62" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI61" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>467</v>
       </c>
@@ -7815,8 +8002,11 @@
       <c r="BH62" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="63" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI62" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>473</v>
       </c>
@@ -7883,8 +8073,11 @@
       <c r="BH63" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="64" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI63" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>479</v>
       </c>
@@ -7951,8 +8144,11 @@
       <c r="BH64" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="65" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI64" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>485</v>
       </c>
@@ -8019,8 +8215,11 @@
       <c r="BH65" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="66" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI65" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>491</v>
       </c>
@@ -8087,8 +8286,11 @@
       <c r="BH66" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="67" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI66" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>497</v>
       </c>
@@ -8155,8 +8357,11 @@
       <c r="BH67" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="68" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI67" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>503</v>
       </c>
@@ -8217,8 +8422,11 @@
       <c r="BH68" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="69" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI68" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>513</v>
       </c>
@@ -8279,8 +8487,11 @@
       <c r="BH69" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="70" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI69" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>520</v>
       </c>
@@ -8341,8 +8552,11 @@
       <c r="BH70" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="71" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI70" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>525</v>
       </c>
@@ -8403,8 +8617,11 @@
       <c r="BH71" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="72" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI71" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>530</v>
       </c>
@@ -8465,8 +8682,11 @@
       <c r="BH72" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="73" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI72" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>535</v>
       </c>
@@ -8527,8 +8747,11 @@
       <c r="BH73" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="74" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI73" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>540</v>
       </c>
@@ -8589,8 +8812,11 @@
       <c r="BH74" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="75" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI74" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>545</v>
       </c>
@@ -8651,8 +8877,11 @@
       <c r="BH75" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="76" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI75" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>549</v>
       </c>
@@ -8713,8 +8942,11 @@
       <c r="BH76" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="77" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI76" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>554</v>
       </c>
@@ -8766,8 +8998,11 @@
       <c r="BH77" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="78" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI77" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>564</v>
       </c>
@@ -8816,8 +9051,11 @@
       <c r="BH78" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="79" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI78" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>571</v>
       </c>
@@ -8878,8 +9116,11 @@
       <c r="BH79" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="80" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI79" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>579</v>
       </c>
@@ -8934,8 +9175,11 @@
       <c r="BH80" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="81" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI80" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>590</v>
       </c>
@@ -8990,8 +9234,11 @@
       <c r="BH81" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="82" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI81" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>603</v>
       </c>
@@ -9049,8 +9296,11 @@
       <c r="BH82" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="83" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI82" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>617</v>
       </c>
@@ -9108,8 +9358,11 @@
       <c r="BH83" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="84" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI83" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>626</v>
       </c>
@@ -9167,8 +9420,11 @@
       <c r="BH84" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="85" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI84" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>634</v>
       </c>
@@ -9223,8 +9479,11 @@
       <c r="BH85" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="86" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI85" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>646</v>
       </c>
@@ -9279,8 +9538,11 @@
       <c r="BH86" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="87" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI86" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>653</v>
       </c>
@@ -9335,8 +9597,11 @@
       <c r="BH87" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="88" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI87" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>660</v>
       </c>
@@ -9409,8 +9674,11 @@
       <c r="BH88" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="89" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI88" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>668</v>
       </c>
@@ -9462,8 +9730,11 @@
       <c r="BH89" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="90" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI89" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>678</v>
       </c>
@@ -9518,8 +9789,11 @@
       <c r="BH90" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="91" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI90" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>686</v>
       </c>
@@ -9574,8 +9848,11 @@
       <c r="BH91" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="92" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI91" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>697</v>
       </c>
@@ -9630,8 +9907,11 @@
       <c r="BH92" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="93" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI92" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>708</v>
       </c>
@@ -9686,8 +9966,11 @@
       <c r="BH93" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="94" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI93" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>716</v>
       </c>
@@ -9808,8 +10091,11 @@
       <c r="BH94" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="95" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI94" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>726</v>
       </c>
@@ -9864,8 +10150,11 @@
       <c r="BH95" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="96" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI95" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>734</v>
       </c>
@@ -9929,8 +10218,11 @@
       <c r="BH96" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="97" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI96" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>742</v>
       </c>
@@ -9985,8 +10277,11 @@
       <c r="BH97" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="98" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI97" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>752</v>
       </c>
@@ -10053,8 +10348,11 @@
       <c r="BH98" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="99" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI98" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>761</v>
       </c>
@@ -10106,8 +10404,11 @@
       <c r="BH99" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="100" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI99" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>770</v>
       </c>
@@ -10159,8 +10460,11 @@
       <c r="BH100" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="101" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI100" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>779</v>
       </c>
@@ -10212,8 +10516,11 @@
       <c r="BH101" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="102" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI101" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>787</v>
       </c>
@@ -10268,8 +10575,11 @@
       <c r="BH102" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="103" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI102" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>795</v>
       </c>
@@ -10324,8 +10634,11 @@
       <c r="BH103" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="104" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI103" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>806</v>
       </c>
@@ -10374,8 +10687,11 @@
       <c r="BH104" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="105" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI104" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>815</v>
       </c>
@@ -10424,8 +10740,11 @@
       <c r="BH105" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="106" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI105" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>822</v>
       </c>
@@ -10489,8 +10808,11 @@
       <c r="BH106" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="107" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI106" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>831</v>
       </c>
@@ -10542,8 +10864,11 @@
       <c r="BH107" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="108" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI107" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>838</v>
       </c>
@@ -10595,8 +10920,11 @@
       <c r="BH108" t="s">
         <v>839</v>
       </c>
-    </row>
-    <row r="109" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI108" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>845</v>
       </c>
@@ -10651,8 +10979,11 @@
       <c r="BH109" t="s">
         <v>846</v>
       </c>
-    </row>
-    <row r="110" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI109" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>856</v>
       </c>
@@ -10716,8 +11047,11 @@
       <c r="BH110" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="111" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI110" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>863</v>
       </c>
@@ -10781,8 +11115,11 @@
       <c r="BH111" t="s">
         <v>870</v>
       </c>
-    </row>
-    <row r="112" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI111" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>871</v>
       </c>
@@ -10840,8 +11177,11 @@
       <c r="BB112" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="113" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI112" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>877</v>
       </c>
@@ -10899,8 +11239,11 @@
       <c r="BB113" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="114" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI113" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>882</v>
       </c>
@@ -10949,8 +11292,11 @@
       <c r="AU114" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="115" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI114" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>889</v>
       </c>
@@ -10999,8 +11345,11 @@
       <c r="AU115" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="116" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI115" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>895</v>
       </c>
@@ -11049,8 +11398,11 @@
       <c r="AU116" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="117" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI116" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>901</v>
       </c>
@@ -11102,8 +11454,11 @@
       <c r="BH117" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="118" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI117" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>908</v>
       </c>
@@ -11164,8 +11519,11 @@
       <c r="BB118" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="119" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI118" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>915</v>
       </c>
@@ -11226,8 +11584,11 @@
       <c r="BC119" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="120" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI119" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>921</v>
       </c>
@@ -11273,8 +11634,11 @@
       <c r="BG120" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="121" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI120" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>930</v>
       </c>
@@ -11326,8 +11690,11 @@
       <c r="BH121" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="122" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI121" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>937</v>
       </c>
@@ -11394,8 +11761,11 @@
       <c r="BH122" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="123" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI122" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>945</v>
       </c>
@@ -11468,8 +11838,11 @@
       <c r="BH123" t="s">
         <v>952</v>
       </c>
-    </row>
-    <row r="124" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI123" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>953</v>
       </c>
@@ -11524,8 +11897,11 @@
       <c r="BH124" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="125" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI124" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>961</v>
       </c>
@@ -11592,8 +11968,11 @@
       <c r="BH125" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="126" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI125" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>970</v>
       </c>
@@ -11645,8 +12024,11 @@
       <c r="BH126" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="127" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI126" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>977</v>
       </c>
@@ -11698,8 +12080,11 @@
       <c r="BH127" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="128" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI127" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>985</v>
       </c>
@@ -11754,8 +12139,11 @@
       <c r="BH128" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="129" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI128" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>995</v>
       </c>
@@ -11810,8 +12198,11 @@
       <c r="BH129" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="130" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI129" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>1005</v>
       </c>
@@ -11866,8 +12257,11 @@
       <c r="BH130" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="131" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI130" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>1013</v>
       </c>
@@ -11922,8 +12316,11 @@
       <c r="BH131" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="132" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI131" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>1023</v>
       </c>
@@ -11978,8 +12375,11 @@
       <c r="BH132" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="133" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI132" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>1030</v>
       </c>
@@ -12034,8 +12434,11 @@
       <c r="BH133" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="134" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI133" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>1038</v>
       </c>
@@ -12090,8 +12493,11 @@
       <c r="BH134" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="135" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI134" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>1045</v>
       </c>
@@ -12146,8 +12552,11 @@
       <c r="BH135" t="s">
         <v>1051</v>
       </c>
-    </row>
-    <row r="136" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI135" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>1052</v>
       </c>
@@ -12201,6 +12610,9 @@
       </c>
       <c r="BH136" t="s">
         <v>1053</v>
+      </c>
+      <c r="BI136" s="4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>